<commit_message>
add modifications to n fertilization treatments to better capture jan/dorian experimental treatments
</commit_message>
<xml_diff>
--- a/projects/jan_dorian_pilot/JanDorian_nFertTreat.xlsx
+++ b/projects/jan_dorian_pilot/JanDorian_nFertTreat.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/lemontree_experimental_wg/projects/jan_dorian_pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46F57844-142A-B54D-B066-1D538A752AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A41375B-8AA2-4746-A9FB-D409F4F5D008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="10180" windowWidth="28120" windowHeight="28300" activeTab="1" xr2:uid="{B491DBE8-45FA-FF4F-853F-7D6D59BE1E36}"/>
+    <workbookView xWindow="2780" yWindow="500" windowWidth="28260" windowHeight="28300" activeTab="1" xr2:uid="{B491DBE8-45FA-FF4F-853F-7D6D59BE1E36}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock solutions" sheetId="1" r:id="rId1"/>
-    <sheet name="58 ppm N, 4 ppm P" sheetId="11" r:id="rId2"/>
-    <sheet name="115 ppm N, 8 ppm P" sheetId="12" r:id="rId3"/>
-    <sheet name="230 ppm N, 15 ppm P" sheetId="8" r:id="rId4"/>
+    <sheet name="Low N" sheetId="8" r:id="rId2"/>
+    <sheet name="Medium N" sheetId="12" r:id="rId3"/>
+    <sheet name="High soil N" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="67">
   <si>
     <t>compound name and stock solution  molarity</t>
   </si>
@@ -1203,9 +1203,6 @@
     <t>moles</t>
   </si>
   <si>
-    <t>ppm (μg/L)</t>
-  </si>
-  <si>
     <t>fert.freq</t>
   </si>
   <si>
@@ -1222,6 +1219,9 @@
   </si>
   <si>
     <t>μg/week</t>
+  </si>
+  <si>
+    <t>mg/plant/8wk</t>
   </si>
 </sst>
 </file>
@@ -1881,20 +1881,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9171829F-9A3B-894F-9068-1544B61E1FDC}">
-  <dimension ref="A1:F45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C438477C-3D1F-8648-B884-34D79DFE18D0}">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1931,11 +1932,11 @@
         <v>115.3</v>
       </c>
       <c r="D3">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="E3" s="3">
         <f>(C3*1000)/(1000/(B3*D3))</f>
-        <v>14.4125</v>
+        <v>11.53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -1985,11 +1986,11 @@
         <v>80.043000000000006</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="3">
         <f>(C6*1000)/(1000/(B6*D6))</f>
-        <v>40.021500000000003</v>
+        <v>8.0043000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2063,7 +2064,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ref="E12" si="0">(C12*1000)/(1000/(B12*D12))</f>
+        <f t="shared" ref="E12:E15" si="0">(C12*1000)/(1000/(B12*D12))</f>
         <v>300.26100000000002</v>
       </c>
     </row>
@@ -2081,7 +2082,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" ref="E13:E15" si="1">(C13*1000)/(1000/(B13*D13))</f>
+        <f t="shared" si="0"/>
         <v>240.732</v>
       </c>
     </row>
@@ -2096,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2111,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2149,11 +2150,11 @@
       </c>
       <c r="D20">
         <f>D3</f>
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="E20" s="3">
         <f>(C20*1000)/(1000/(B20*D20))</f>
-        <v>1.75075</v>
+        <v>1.4006000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2168,11 +2169,11 @@
       </c>
       <c r="D21">
         <f>D3</f>
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" ref="E21:E33" si="2">(C21*1000)/(1000/(B21*D21))</f>
-        <v>3.8717125000000001</v>
+        <f t="shared" ref="E21:E33" si="1">(C21*1000)/(1000/(B21*D21))</f>
+        <v>3.0973700000000002</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2190,7 +2191,7 @@
         <v>0.5</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>39.094299999999997</v>
       </c>
     </row>
@@ -2228,7 +2229,7 @@
         <v>0.5</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40.078000000000003</v>
       </c>
     </row>
@@ -2247,7 +2248,7 @@
         <v>0.5</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28.012</v>
       </c>
     </row>
@@ -2263,11 +2264,11 @@
       </c>
       <c r="D26">
         <f>D6</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="2"/>
-        <v>14.006</v>
+        <f t="shared" si="1"/>
+        <v>2.8012000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2321,7 +2322,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>117.2829</v>
       </c>
     </row>
@@ -2340,7 +2341,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>106.35900000000001</v>
       </c>
     </row>
@@ -2359,7 +2360,7 @@
         <v>3</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>120.23400000000001</v>
       </c>
     </row>
@@ -2378,11 +2379,11 @@
         <v>1</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>48.61</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2397,88 +2398,99 @@
         <v>1</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>64.13</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>51</v>
       </c>
       <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" t="s">
         <v>64</v>
       </c>
-      <c r="C37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>65</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="3">
         <f>SUM(E20,E23,E25,E26)</f>
-        <v>57.774749999999997</v>
+        <v>46.219799999999999</v>
       </c>
       <c r="C38" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D38" s="11">
-        <v>2</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
       </c>
       <c r="E38" s="3">
         <f>B38*C38*D38</f>
-        <v>17.332424999999997</v>
+        <v>3.466485</v>
       </c>
       <c r="F38" s="11">
         <f>E38*1000</f>
-        <v>17332.424999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3466.4850000000001</v>
+      </c>
+      <c r="G38" s="3">
+        <f>E38*8</f>
+        <v>27.73188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
       <c r="B39" s="3">
         <f>SUM(E21,E28)</f>
-        <v>3.8717125000000001</v>
+        <v>3.0973700000000002</v>
       </c>
       <c r="C39" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D39" s="11">
-        <v>2</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" ref="E39:E43" si="3">B39*C39*D39</f>
-        <v>1.1615137499999999</v>
+        <f t="shared" ref="E39:E43" si="2">B39*C39*D39</f>
+        <v>0.23230275</v>
       </c>
       <c r="F39" s="11">
-        <f t="shared" ref="F39:F43" si="4">E39*1000</f>
-        <v>1161.5137499999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F39:F43" si="3">E39*1000</f>
+        <v>232.30275</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" ref="G39:G43" si="4">E39*8</f>
+        <v>1.858422</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2487,21 +2499,25 @@
         <v>156.37719999999999</v>
       </c>
       <c r="C40" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D40" s="11">
-        <v>2</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
       </c>
       <c r="E40" s="3">
+        <f t="shared" si="2"/>
+        <v>11.728289999999999</v>
+      </c>
+      <c r="F40" s="11">
         <f t="shared" si="3"/>
-        <v>46.913159999999998</v>
-      </c>
-      <c r="F40" s="11">
+        <v>11728.289999999999</v>
+      </c>
+      <c r="G40" s="3">
         <f t="shared" si="4"/>
-        <v>46913.159999999996</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>93.826319999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2510,21 +2526,25 @@
         <v>160.31200000000001</v>
       </c>
       <c r="C41" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D41" s="11">
-        <v>2</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
       </c>
       <c r="E41" s="3">
+        <f t="shared" si="2"/>
+        <v>12.023400000000001</v>
+      </c>
+      <c r="F41" s="11">
         <f t="shared" si="3"/>
-        <v>48.093600000000002</v>
-      </c>
-      <c r="F41" s="11">
+        <v>12023.4</v>
+      </c>
+      <c r="G41" s="3">
         <f t="shared" si="4"/>
-        <v>48093.599999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>96.187200000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2533,21 +2553,25 @@
         <v>48.61</v>
       </c>
       <c r="C42" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D42" s="11">
-        <v>2</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
       </c>
       <c r="E42" s="3">
+        <f t="shared" si="2"/>
+        <v>3.6457499999999996</v>
+      </c>
+      <c r="F42" s="11">
         <f t="shared" si="3"/>
-        <v>14.582999999999998</v>
-      </c>
-      <c r="F42" s="11">
+        <v>3645.7499999999995</v>
+      </c>
+      <c r="G42" s="3">
         <f t="shared" si="4"/>
-        <v>14582.999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>29.165999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2556,27 +2580,31 @@
         <v>64.13</v>
       </c>
       <c r="C43" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D43" s="11">
-        <v>2</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
       </c>
       <c r="E43" s="3">
+        <f t="shared" si="2"/>
+        <v>4.8097499999999993</v>
+      </c>
+      <c r="F43" s="11">
         <f t="shared" si="3"/>
-        <v>19.238999999999997</v>
-      </c>
-      <c r="F43" s="11">
+        <v>4809.7499999999991</v>
+      </c>
+      <c r="G43" s="3">
         <f t="shared" si="4"/>
-        <v>19238.999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>38.477999999999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="13">
-        <f>B38/B39</f>
+        <f>G38/G39</f>
         <v>14.922272766895786</v>
       </c>
     </row>
@@ -2587,10 +2615,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436DBBC1-A853-6941-AE23-466C19224FD0}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2638,11 +2666,11 @@
         <v>115.3</v>
       </c>
       <c r="D3">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="E3" s="3">
         <f>(C3*1000)/(1000/(B3*D3))</f>
-        <v>28.824999999999999</v>
+        <v>11.53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2656,11 +2684,11 @@
         <v>101.1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="3">
         <f>(C4*1000)/(1000/(B4*D4))</f>
-        <v>202.2</v>
+        <v>101.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2674,11 +2702,11 @@
         <v>164.08799999999999</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="3">
         <f>(C5*1000)/(1000/(B5*D5))</f>
-        <v>328.17599999999999</v>
+        <v>164.08799999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2692,11 +2720,11 @@
         <v>80.043000000000006</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="3">
         <f>(C6*1000)/(1000/(B6*D6))</f>
-        <v>80.043000000000006</v>
+        <v>8.0043000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2749,11 +2777,11 @@
         <v>74.555000000000007</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
         <f>(C11*1000)/(1000/(B11*D11))</f>
-        <v>149.11000000000001</v>
+        <v>223.66500000000002</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2767,11 +2795,11 @@
         <v>100.087</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ref="E12:E15" si="0">(C12*1000)/(1000/(B12*D12))</f>
-        <v>200.17400000000001</v>
+        <v>300.26100000000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2856,11 +2884,11 @@
       </c>
       <c r="D20">
         <f>D3</f>
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="E20" s="3">
         <f>(C20*1000)/(1000/(B20*D20))</f>
-        <v>3.5015000000000001</v>
+        <v>1.4006000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2875,11 +2903,11 @@
       </c>
       <c r="D21">
         <f>D3</f>
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ref="E21:E33" si="1">(C21*1000)/(1000/(B21*D21))</f>
-        <v>7.7434250000000002</v>
+        <v>3.0973700000000002</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2894,11 +2922,11 @@
       </c>
       <c r="D22">
         <f>D4</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="1"/>
-        <v>78.188599999999994</v>
+        <v>39.094299999999997</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2913,11 +2941,11 @@
       </c>
       <c r="D23">
         <f>D4</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="3">
         <f>(C23*1000)/(1000/(B23*D23))</f>
-        <v>28.012</v>
+        <v>14.006</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2932,11 +2960,11 @@
       </c>
       <c r="D24">
         <f>D5</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" si="1"/>
-        <v>80.156000000000006</v>
+        <v>40.078000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2951,11 +2979,11 @@
       </c>
       <c r="D25">
         <f>D5</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="1"/>
-        <v>56.024000000000001</v>
+        <v>28.012</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2970,11 +2998,11 @@
       </c>
       <c r="D26">
         <f>D6</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="1"/>
-        <v>28.012</v>
+        <v>2.8012000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3025,11 +3053,11 @@
       </c>
       <c r="D29">
         <f>D11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>78.188599999999994</v>
+        <v>117.2829</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3044,11 +3072,11 @@
       </c>
       <c r="D30">
         <f>D11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" si="1"/>
-        <v>70.906000000000006</v>
+        <v>106.35900000000001</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3063,11 +3091,11 @@
       </c>
       <c r="D31">
         <f>D12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="3">
         <f t="shared" si="1"/>
-        <v>80.156000000000006</v>
+        <v>120.23400000000001</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3089,7 +3117,7 @@
         <v>48.61</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -3108,84 +3136,95 @@
         <v>64.13</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>51</v>
       </c>
       <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
         <v>60</v>
       </c>
-      <c r="C37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" t="s">
-        <v>61</v>
-      </c>
       <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="s">
         <v>65</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="3">
         <f>SUM(E20,E23,E25,E26)</f>
-        <v>115.54949999999999</v>
+        <v>46.219799999999999</v>
       </c>
       <c r="C38" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D38" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="3">
         <f>B38*C38*D38</f>
-        <v>34.664849999999994</v>
+        <v>4.6219799999999998</v>
       </c>
       <c r="F38" s="11">
         <f>E38*1000</f>
-        <v>34664.849999999991</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4621.9799999999996</v>
+      </c>
+      <c r="G38" s="3">
+        <f>E38*8</f>
+        <v>36.975839999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
       <c r="B39" s="3">
         <f>SUM(E21,E28)</f>
-        <v>7.7434250000000002</v>
+        <v>3.0973700000000002</v>
       </c>
       <c r="C39" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D39" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" ref="E39:E43" si="2">B39*C39*D39</f>
-        <v>2.3230274999999998</v>
+        <v>0.30973700000000004</v>
       </c>
       <c r="F39" s="11">
         <f t="shared" ref="F39:F43" si="3">E39*1000</f>
-        <v>2323.0274999999997</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>309.73700000000002</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" ref="G39:G43" si="4">E39*8</f>
+        <v>2.4778960000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3194,21 +3233,25 @@
         <v>156.37719999999999</v>
       </c>
       <c r="C40" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D40" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" si="2"/>
-        <v>46.913159999999998</v>
+        <v>15.63772</v>
       </c>
       <c r="F40" s="11">
         <f t="shared" si="3"/>
-        <v>46913.159999999996</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15637.72</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="4"/>
+        <v>125.10176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3217,21 +3260,25 @@
         <v>160.31200000000001</v>
       </c>
       <c r="C41" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D41" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" si="2"/>
-        <v>48.093600000000002</v>
+        <v>16.031200000000002</v>
       </c>
       <c r="F41" s="11">
         <f t="shared" si="3"/>
-        <v>48093.599999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16031.200000000003</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="4"/>
+        <v>128.24960000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -3240,21 +3287,25 @@
         <v>48.61</v>
       </c>
       <c r="C42" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D42" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="3">
         <f t="shared" si="2"/>
-        <v>14.582999999999998</v>
+        <v>4.8610000000000007</v>
       </c>
       <c r="F42" s="11">
         <f t="shared" si="3"/>
-        <v>14582.999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4861.0000000000009</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="4"/>
+        <v>38.888000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -3263,28 +3314,32 @@
         <v>64.13</v>
       </c>
       <c r="C43" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D43" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" si="2"/>
-        <v>19.238999999999997</v>
+        <v>6.4130000000000003</v>
       </c>
       <c r="F43" s="11">
         <f t="shared" si="3"/>
-        <v>19238.999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6413</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="4"/>
+        <v>51.304000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="13">
-        <f>B38/B39</f>
-        <v>14.922272766895786</v>
+        <f>G38/G39</f>
+        <v>14.922272766895784</v>
       </c>
     </row>
   </sheetData>
@@ -3293,20 +3348,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C438477C-3D1F-8648-B884-34D79DFE18D0}">
-  <dimension ref="A1:F45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9171829F-9A3B-894F-9068-1544B61E1FDC}">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A32" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -3343,11 +3400,11 @@
         <v>115.3</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E3" s="3">
         <f>(C3*1000)/(1000/(B3*D3))</f>
-        <v>57.65</v>
+        <v>11.53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3361,11 +3418,11 @@
         <v>101.1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="3">
         <f>(C4*1000)/(1000/(B4*D4))</f>
-        <v>404.4</v>
+        <v>101.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3379,11 +3436,11 @@
         <v>164.08799999999999</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="3">
         <f>(C5*1000)/(1000/(B5*D5))</f>
-        <v>656.35199999999998</v>
+        <v>164.08799999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3397,11 +3454,11 @@
         <v>80.043000000000006</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="3">
         <f>(C6*1000)/(1000/(B6*D6))</f>
-        <v>160.08600000000001</v>
+        <v>8.0043000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3454,10 +3511,11 @@
         <v>74.555000000000007</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
-        <v>0</v>
+        <f>(C11*1000)/(1000/(B11*D11))</f>
+        <v>223.66500000000002</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3471,10 +3529,11 @@
         <v>100.087</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <f t="shared" ref="E12" si="0">(C12*1000)/(1000/(B12*D12))</f>
+        <v>300.26100000000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3491,7 +3550,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" ref="E13" si="0">(C13*1000)/(1000/(B13*D13))</f>
+        <f t="shared" ref="E13:E15" si="1">(C13*1000)/(1000/(B13*D13))</f>
         <v>240.732</v>
       </c>
     </row>
@@ -3506,7 +3565,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" ref="E14:E15" si="1">(C14*1000)/(1000/(B14*D14))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3525,12 +3584,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3547,7 +3606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -3559,15 +3618,14 @@
       </c>
       <c r="D20">
         <f>D3</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E20" s="3">
         <f>(C20*1000)/(1000/(B20*D20))</f>
-        <v>7.0030000000000001</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>1.4006000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -3579,15 +3637,14 @@
       </c>
       <c r="D21">
         <f>D3</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" ref="E21:E33" si="2">(C21*1000)/(1000/(B21*D21))</f>
-        <v>15.48685</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>3.0973700000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -3599,15 +3656,14 @@
       </c>
       <c r="D22">
         <f>D4</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="2"/>
-        <v>156.37719999999999</v>
-      </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>39.094299999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -3619,15 +3675,14 @@
       </c>
       <c r="D23">
         <f>D4</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="3">
         <f>(C23*1000)/(1000/(B23*D23))</f>
-        <v>56.024000000000001</v>
-      </c>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>14.006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -3639,15 +3694,14 @@
       </c>
       <c r="D24">
         <f>D5</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" si="2"/>
-        <v>160.31200000000001</v>
-      </c>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>40.078000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -3659,15 +3713,14 @@
       </c>
       <c r="D25">
         <f>D5</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="2"/>
-        <v>112.048</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>28.012</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -3679,15 +3732,14 @@
       </c>
       <c r="D26">
         <f>D6</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="2"/>
-        <v>56.024000000000001</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>2.8012000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -3704,9 +3756,8 @@
       <c r="E27" s="3">
         <v>0</v>
       </c>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -3723,9 +3774,8 @@
       <c r="E28" s="3">
         <v>0</v>
       </c>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -3737,14 +3787,14 @@
       </c>
       <c r="D29">
         <f>D11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E29" s="3">
-        <v>0</v>
-      </c>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>117.2829</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -3756,14 +3806,14 @@
       </c>
       <c r="D30">
         <f>D11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>106.35900000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -3775,14 +3825,14 @@
       </c>
       <c r="D31">
         <f>D12</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
-      </c>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>120.23400000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -3800,9 +3850,8 @@
         <f t="shared" si="2"/>
         <v>48.61</v>
       </c>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -3820,86 +3869,96 @@
         <f t="shared" si="2"/>
         <v>64.13</v>
       </c>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>51</v>
       </c>
       <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
         <v>60</v>
       </c>
-      <c r="C37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" t="s">
-        <v>61</v>
-      </c>
       <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="s">
         <v>65</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="3">
         <f>SUM(E20,E23,E25,E26)</f>
-        <v>231.09899999999999</v>
+        <v>46.219799999999999</v>
       </c>
       <c r="C38" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D38" s="11">
         <v>2</v>
       </c>
       <c r="E38" s="3">
         <f>B38*C38*D38</f>
-        <v>69.329699999999988</v>
+        <v>9.2439599999999995</v>
       </c>
       <c r="F38" s="11">
         <f>E38*1000</f>
-        <v>69329.699999999983</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9243.9599999999991</v>
+      </c>
+      <c r="G38" s="3">
+        <f>E38*8</f>
+        <v>73.951679999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
       <c r="B39" s="3">
         <f>SUM(E21,E28)</f>
-        <v>15.48685</v>
+        <v>3.0973700000000002</v>
       </c>
       <c r="C39" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D39" s="11">
         <v>2</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" ref="E39:E43" si="3">B39*C39*D39</f>
-        <v>4.6460549999999996</v>
+        <v>0.61947400000000008</v>
       </c>
       <c r="F39" s="11">
         <f t="shared" ref="F39:F43" si="4">E39*1000</f>
-        <v>4646.0549999999994</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>619.47400000000005</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" ref="G39:G43" si="5">E39*8</f>
+        <v>4.9557920000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3908,21 +3967,25 @@
         <v>156.37719999999999</v>
       </c>
       <c r="C40" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D40" s="11">
         <v>2</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" si="3"/>
-        <v>46.913159999999998</v>
+        <v>31.27544</v>
       </c>
       <c r="F40" s="11">
         <f t="shared" si="4"/>
-        <v>46913.159999999996</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31275.439999999999</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="5"/>
+        <v>250.20352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3931,21 +3994,25 @@
         <v>160.31200000000001</v>
       </c>
       <c r="C41" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D41" s="11">
         <v>2</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" si="3"/>
-        <v>48.093600000000002</v>
+        <v>32.062400000000004</v>
       </c>
       <c r="F41" s="11">
         <f t="shared" si="4"/>
-        <v>48093.599999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32062.400000000005</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="5"/>
+        <v>256.49920000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -3954,21 +4021,25 @@
         <v>48.61</v>
       </c>
       <c r="C42" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D42" s="11">
         <v>2</v>
       </c>
       <c r="E42" s="3">
         <f t="shared" si="3"/>
-        <v>14.582999999999998</v>
+        <v>9.7220000000000013</v>
       </c>
       <c r="F42" s="11">
         <f t="shared" si="4"/>
-        <v>14582.999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9722.0000000000018</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="5"/>
+        <v>77.77600000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -3977,28 +4048,32 @@
         <v>64.13</v>
       </c>
       <c r="C43" s="10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D43" s="11">
         <v>2</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" si="3"/>
-        <v>19.238999999999997</v>
+        <v>12.826000000000001</v>
       </c>
       <c r="F43" s="11">
         <f t="shared" si="4"/>
-        <v>19238.999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>12826</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="5"/>
+        <v>102.608</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="13">
-        <f>B38/B39</f>
-        <v>14.922272766895786</v>
+        <f>G38/G39</f>
+        <v>14.922272766895784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>